<commit_message>
final updation of the product
</commit_message>
<xml_diff>
--- a/src/excel/Project Enquiry Register - 18-19 Template.xlsx
+++ b/src/excel/Project Enquiry Register - 18-19 Template.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Client Details" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet sheetId="1" name="Sheet1" r:id="rId4"/>
+    <sheet sheetId="3" name="Client Details" r:id="rId5"/>
+    <sheet sheetId="4" name="Sheet2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase">Sheet1!$A$4:$AA$24</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!A1:AA3</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="147">
   <si>
     <t xml:space="preserve"> ENQUIRY REGISTER - 2018 - 2019 FOR PROJECTS</t>
   </si>
@@ -450,55 +450,70 @@
   </si>
   <si>
     <t>jhhjj</t>
+  </si>
+  <si>
+    <t>kkkkkkkkk</t>
+  </si>
+  <si>
+    <t>retort</t>
+  </si>
+  <si>
+    <t>kljlkjlkjklj</t>
+  </si>
+  <si>
+    <t>kljjkl</t>
+  </si>
+  <si>
+    <t>lkjjkl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * -#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ [$₹-4009] * #,##0.00_ ;_ [$₹-4009] * -#,##0.00_ ;_ [$₹-4009] * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* -#,##0.00 ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="6">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <family val="1"/>
       <sz val="10"/>
       <name val="Book Antiqua"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <family val="1"/>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Book Antiqua"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
+      <family val="1"/>
       <sz val="10"/>
       <name val="Book Antiqua"/>
-      <family val="1"/>
     </font>
     <font>
+      <color theme="1"/>
+      <family val="1"/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Book Antiqua"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -553,16 +568,16 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,27 +594,27 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="0" tint="-0.1499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,16 +633,16 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+        <color theme="0" tint="-0.249946592608417"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+        <color theme="0" tint="-0.249946592608417"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+        <color theme="0" tint="-0.249946592608417"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+        <color theme="0" tint="-0.249946592608417"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -646,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -658,10 +673,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -673,10 +691,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -688,7 +709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -700,7 +721,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -718,10 +739,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -733,7 +754,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -745,19 +766,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,15 +1049,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="2" customWidth="1"/>
@@ -1072,937 +1084,936 @@
     <col min="25" max="26" width="12.140625" style="1" customWidth="1"/>
     <col min="27" max="27" width="23.7109375" style="3" customWidth="1"/>
     <col min="28" max="28" width="11" style="6" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="6" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="6"/>
+    <col min="29" max="16384" width="9.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="9" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" ht="16.5" customHeight="1" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="10"/>
-    </row>
-    <row r="2" spans="1:28" s="11" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="11"/>
+    </row>
+    <row r="2" ht="30" customHeight="1" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40" t="s">
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="13"/>
-    </row>
-    <row r="3" spans="1:28" s="11" customFormat="1" ht="60" customHeight="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="12" t="s">
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="15"/>
+    </row>
+    <row r="3" ht="60" customHeight="1" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="X3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Y3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AB3" s="13"/>
-    </row>
-    <row r="4" spans="1:28">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="17"/>
-      <c r="AB4" s="23"/>
-    </row>
-    <row r="5" spans="1:28" ht="16.5" customHeight="1">
-      <c r="A5" s="15" t="s">
+      <c r="AB3" s="15"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="25"/>
+    </row>
+    <row r="5" ht="16.5" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="17" t="s">
+      <c r="J5" s="17"/>
+      <c r="K5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="15" t="s">
+      <c r="N5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="22">
+      <c r="O5" s="24">
         <v>111111</v>
       </c>
-      <c r="P5" s="22">
+      <c r="P5" s="24">
         <f>O5</f>
         <v>111111</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="24"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15" t="s">
+      <c r="R5" s="26"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AA5" s="15" t="s">
+      <c r="AA5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" s="23"/>
-    </row>
-    <row r="6" spans="1:28" ht="16.5" customHeight="1">
-      <c r="A6" s="15" t="s">
+      <c r="AB5" s="25"/>
+    </row>
+    <row r="6" ht="16.5" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="20">
         <v>222222</v>
       </c>
-      <c r="P6" s="22">
+      <c r="P6" s="24">
         <f t="shared" ref="P6:P7" si="0">O6</f>
         <v>222222</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="24"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15" t="s">
+      <c r="R6" s="26"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AA6" s="15" t="s">
+      <c r="AA6" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AB6" s="23"/>
-    </row>
-    <row r="7" spans="1:28" ht="16.5" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="AB6" s="25"/>
+    </row>
+    <row r="7" ht="16.5" customHeight="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="20">
         <v>333333</v>
       </c>
-      <c r="P7" s="22">
+      <c r="P7" s="24">
         <f t="shared" si="0"/>
         <v>333333</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="Q7" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="R7" s="24"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15" t="s">
+      <c r="R7" s="26"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AA7" s="15" t="s">
+      <c r="AA7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AB7" s="23"/>
-    </row>
-    <row r="8" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="26"/>
-    </row>
-    <row r="9" spans="1:28" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="26"/>
-    </row>
-    <row r="10" spans="1:28" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="26"/>
-    </row>
-    <row r="11" spans="1:28" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="26"/>
-    </row>
-    <row r="12" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="26"/>
-    </row>
-    <row r="13" spans="1:28" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="26"/>
-    </row>
-    <row r="14" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="26"/>
-    </row>
-    <row r="15" spans="1:28" s="25" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="26"/>
-    </row>
-    <row r="16" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
-      <c r="AB16" s="26"/>
-    </row>
-    <row r="17" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="15"/>
-      <c r="AB17" s="26"/>
-    </row>
-    <row r="18" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="26"/>
-    </row>
-    <row r="19" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
-      <c r="AA19" s="15"/>
-      <c r="AB19" s="26"/>
-    </row>
-    <row r="20" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-      <c r="AA20" s="15"/>
-      <c r="AB20" s="26"/>
-    </row>
-    <row r="21" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
-      <c r="AA21" s="15"/>
-      <c r="AB21" s="26"/>
-    </row>
-    <row r="22" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="26"/>
-    </row>
-    <row r="23" spans="1:28" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-      <c r="AA23" s="15"/>
-      <c r="AB23" s="26"/>
-    </row>
-    <row r="24" spans="1:28" s="25" customFormat="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="21"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="22"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
-      <c r="AA24" s="17"/>
-      <c r="AB24" s="26"/>
-    </row>
-    <row r="25" spans="1:28">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="32"/>
-      <c r="S25" s="35"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="36"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="37"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="32"/>
-    </row>
-    <row r="26" spans="1:28">
+      <c r="AB7" s="25"/>
+    </row>
+    <row r="8" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="28"/>
+    </row>
+    <row r="9" ht="30" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="28"/>
+    </row>
+    <row r="10" ht="30" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="28"/>
+    </row>
+    <row r="11" ht="30" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="28"/>
+    </row>
+    <row r="12" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="28"/>
+    </row>
+    <row r="13" ht="30" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="28"/>
+    </row>
+    <row r="14" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="28"/>
+    </row>
+    <row r="15" ht="30" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="28"/>
+    </row>
+    <row r="16" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="28"/>
+    </row>
+    <row r="17" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="28"/>
+    </row>
+    <row r="18" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="28"/>
+    </row>
+    <row r="19" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="28"/>
+    </row>
+    <row r="20" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="28"/>
+    </row>
+    <row r="21" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="17"/>
+      <c r="AA21" s="17"/>
+      <c r="AB21" s="28"/>
+    </row>
+    <row r="22" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="17"/>
+      <c r="X22" s="17"/>
+      <c r="Y22" s="17"/>
+      <c r="Z22" s="17"/>
+      <c r="AA22" s="17"/>
+      <c r="AB22" s="28"/>
+    </row>
+    <row r="23" ht="16.5" customHeight="1" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="26"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="17"/>
+      <c r="AA23" s="17"/>
+      <c r="AB23" s="28"/>
+    </row>
+    <row r="24" spans="1:28" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="28"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="39"/>
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="32"/>
+      <c r="AA25" s="34"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>64</v>
       </c>
@@ -2010,7 +2021,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>64</v>
       </c>
@@ -2018,7 +2029,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
@@ -2026,7 +2037,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
@@ -2034,7 +2045,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
@@ -2042,7 +2053,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
@@ -2050,7 +2061,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>64</v>
       </c>
@@ -2058,7 +2069,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -2066,7 +2077,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -2074,7 +2085,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>64</v>
       </c>
@@ -2082,7 +2093,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -2102,26 +2113,26 @@
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
   </mergeCells>
-  <pageMargins left="0.2" right="0.19685039370078741" top="0.39370078740157483" bottom="0.27559055118110237" header="0.19685039370078741" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="65" orientation="landscape" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="1200"/>
+  <pageMargins left="0.2" right="0.1968503937007874" top="0.3937007874015748" bottom="0.2755905511811024" header="0.1968503937007874" footer="0.1968503937007874"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="1200" scale="65" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2129,17 +2140,17 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -2147,7 +2158,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>72</v>
       </c>
@@ -2155,7 +2166,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -2163,7 +2174,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -2171,7 +2182,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2184,401 +2195,401 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA48"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0"/>
   <cols>
     <col min="8" max="8" width="28" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40" t="s">
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-    </row>
-    <row r="3" spans="1:27" ht="60" customHeight="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="12" t="s">
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+    </row>
+    <row r="3" ht="60" customHeight="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="X3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Y3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="17"/>
-    </row>
-    <row r="5" spans="1:27" ht="30" customHeight="1">
-      <c r="A5" s="15" t="s">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="19"/>
+    </row>
+    <row r="5" ht="30" customHeight="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="17" t="s">
+      <c r="J5" s="17"/>
+      <c r="K5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="15" t="s">
+      <c r="N5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="22">
+      <c r="O5" s="24">
         <v>111111</v>
       </c>
-      <c r="P5" s="22" t="e">
+      <c r="P5" s="24" t="e">
         <f>B11O5</f>
         <v>#NAME?</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="24"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15" t="s">
+      <c r="R5" s="26"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AA5" s="15" t="s">
+      <c r="AA5" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="45" customHeight="1">
-      <c r="A6" s="15" t="s">
+    <row r="6" ht="45" customHeight="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="20">
         <v>222222</v>
       </c>
-      <c r="P6" s="22">
+      <c r="P6" s="24">
         <f t="shared" ref="P6:P7" si="0">O6</f>
         <v>222222</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="24"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15" t="s">
+      <c r="R6" s="26"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AA6" s="15" t="s">
+      <c r="AA6" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="30" customHeight="1">
-      <c r="A7" s="15" t="s">
+    <row r="7" ht="30" customHeight="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="20">
         <v>333333</v>
       </c>
-      <c r="P7" s="22">
+      <c r="P7" s="24">
         <f t="shared" si="0"/>
         <v>333333</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="Q7" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="R7" s="24"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15" t="s">
+      <c r="R7" s="26"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AA7" s="15" t="s">
+      <c r="AA7" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2600,8 +2611,8 @@
       <c r="G8" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="38">
-        <v>43229.519106087959</v>
+      <c r="H8" s="40">
+        <v>43229.51910608796</v>
       </c>
       <c r="I8" t="s">
         <v>81</v>
@@ -2661,7 +2672,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2683,8 +2694,8 @@
       <c r="G9" t="s">
         <v>80</v>
       </c>
-      <c r="H9" s="38">
-        <v>43229.519363206018</v>
+      <c r="H9" s="40">
+        <v>43229.51936320602</v>
       </c>
       <c r="I9" t="s">
         <v>81</v>
@@ -2744,7 +2755,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2766,8 +2777,8 @@
       <c r="G10" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="38">
-        <v>43229.531475706019</v>
+      <c r="H10" s="40">
+        <v>43229.53147570602</v>
       </c>
       <c r="I10" t="s">
         <v>86</v>
@@ -2827,7 +2838,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -2849,8 +2860,8 @@
       <c r="G11" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="38">
-        <v>43231.174696944443</v>
+      <c r="H11" s="40">
+        <v>43231.17469694444</v>
       </c>
       <c r="I11" t="s">
         <v>88</v>
@@ -2910,7 +2921,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2932,8 +2943,8 @@
       <c r="G12" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="38">
-        <v>43231.179197546298</v>
+      <c r="H12" s="40">
+        <v>43231.1791975463</v>
       </c>
       <c r="I12" t="s">
         <v>88</v>
@@ -2993,7 +3004,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -3015,7 +3026,7 @@
       <c r="G13" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="40">
         <v>43231.179508877314</v>
       </c>
       <c r="I13" t="s">
@@ -3076,7 +3087,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3098,8 +3109,8 @@
       <c r="G14" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="38">
-        <v>43231.182507372687</v>
+      <c r="H14" s="40">
+        <v>43231.18250737269</v>
       </c>
       <c r="I14" t="s">
         <v>88</v>
@@ -3159,7 +3170,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -3181,7 +3192,7 @@
       <c r="G15" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="40">
         <v>43231.185189131946</v>
       </c>
       <c r="I15" t="s">
@@ -3242,7 +3253,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3264,8 +3275,8 @@
       <c r="G16" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="38">
-        <v>43231.198283506943</v>
+      <c r="H16" s="40">
+        <v>43231.19828350694</v>
       </c>
       <c r="I16" t="s">
         <v>95</v>
@@ -3325,7 +3336,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -3347,8 +3358,8 @@
       <c r="G17" t="s">
         <v>80</v>
       </c>
-      <c r="H17" s="38">
-        <v>43231.202369479171</v>
+      <c r="H17" s="40">
+        <v>43231.20236947917</v>
       </c>
       <c r="I17" t="s">
         <v>97</v>
@@ -3408,7 +3419,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -3430,11 +3441,11 @@
       <c r="G18" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="38">
-        <v>43231.209715972218</v>
-      </c>
-      <c r="I18" s="38">
-        <v>25569.000023217592</v>
+      <c r="H18" s="40">
+        <v>43231.20971597222</v>
+      </c>
+      <c r="I18" s="40">
+        <v>25569.00002321759</v>
       </c>
       <c r="J18" t="s">
         <v>76</v>
@@ -3491,7 +3502,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -3513,8 +3524,8 @@
       <c r="G19" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="38">
-        <v>43231.221264305554</v>
+      <c r="H19" s="40">
+        <v>43231.22126430555</v>
       </c>
       <c r="I19" t="s">
         <v>95</v>
@@ -3574,7 +3585,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -3596,8 +3607,8 @@
       <c r="G20" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="38">
-        <v>43231.222943842593</v>
+      <c r="H20" s="40">
+        <v>43231.22294384259</v>
       </c>
       <c r="I20" t="s">
         <v>103</v>
@@ -3657,7 +3668,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -3679,8 +3690,8 @@
       <c r="G21" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="38">
-        <v>43231.228480775462</v>
+      <c r="H21" s="40">
+        <v>43231.22848077546</v>
       </c>
       <c r="I21" t="s">
         <v>105</v>
@@ -3740,7 +3751,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -3762,8 +3773,8 @@
       <c r="G22" t="s">
         <v>80</v>
       </c>
-      <c r="H22" s="38">
-        <v>43231.232120405097</v>
+      <c r="H22" s="40">
+        <v>43231.2321204051</v>
       </c>
       <c r="I22" t="s">
         <v>105</v>
@@ -3823,7 +3834,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3845,7 +3856,7 @@
       <c r="G23" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="40">
         <v>43231.2325991088</v>
       </c>
       <c r="I23" t="s">
@@ -3906,7 +3917,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -3928,8 +3939,8 @@
       <c r="G24" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="38">
-        <v>43231.233160162039</v>
+      <c r="H24" s="40">
+        <v>43231.23316016204</v>
       </c>
       <c r="I24" t="s">
         <v>105</v>
@@ -3989,7 +4000,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -4011,8 +4022,8 @@
       <c r="G25" t="s">
         <v>80</v>
       </c>
-      <c r="H25" s="38">
-        <v>43231.236218194448</v>
+      <c r="H25" s="40">
+        <v>43231.23621819445</v>
       </c>
       <c r="I25" t="s">
         <v>105</v>
@@ -4072,7 +4083,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -4094,7 +4105,7 @@
       <c r="G26" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="38">
+      <c r="H26" s="40">
         <v>43231.239412916664</v>
       </c>
       <c r="I26" t="s">
@@ -4155,7 +4166,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -4177,8 +4188,8 @@
       <c r="G27" t="s">
         <v>80</v>
       </c>
-      <c r="H27" s="38">
-        <v>43231.239453460643</v>
+      <c r="H27" s="40">
+        <v>43231.23945346064</v>
       </c>
       <c r="I27" t="s">
         <v>105</v>
@@ -4238,7 +4249,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -4260,8 +4271,8 @@
       <c r="G28" t="s">
         <v>80</v>
       </c>
-      <c r="H28" s="38">
-        <v>43231.240277083329</v>
+      <c r="H28" s="40">
+        <v>43231.24027708333</v>
       </c>
       <c r="I28" t="s">
         <v>105</v>
@@ -4321,7 +4332,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -4343,8 +4354,8 @@
       <c r="G29" t="s">
         <v>80</v>
       </c>
-      <c r="H29" s="38">
-        <v>43231.240595416668</v>
+      <c r="H29" s="40">
+        <v>43231.24059541667</v>
       </c>
       <c r="I29" t="s">
         <v>105</v>
@@ -4404,7 +4415,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -4426,8 +4437,8 @@
       <c r="G30" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="38">
-        <v>43231.240604849532</v>
+      <c r="H30" s="40">
+        <v>43231.24060484953</v>
       </c>
       <c r="I30" t="s">
         <v>105</v>
@@ -4487,7 +4498,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -4509,8 +4520,8 @@
       <c r="G31" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="38">
-        <v>43231.240610590277</v>
+      <c r="H31" s="40">
+        <v>43231.24061059028</v>
       </c>
       <c r="I31" t="s">
         <v>105</v>
@@ -4570,7 +4581,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -4592,8 +4603,8 @@
       <c r="G32" t="s">
         <v>80</v>
       </c>
-      <c r="H32" s="38">
-        <v>43231.240614201393</v>
+      <c r="H32" s="40">
+        <v>43231.24061420139</v>
       </c>
       <c r="I32" t="s">
         <v>105</v>
@@ -4653,7 +4664,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -4675,7 +4686,7 @@
       <c r="G33" t="s">
         <v>80</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="40">
         <v>43231.240617523144</v>
       </c>
       <c r="I33" t="s">
@@ -4736,7 +4747,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -4758,7 +4769,7 @@
       <c r="G34" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="40">
         <v>43231.242404756944</v>
       </c>
       <c r="I34" t="s">
@@ -4819,7 +4830,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -4841,7 +4852,7 @@
       <c r="G35" t="s">
         <v>80</v>
       </c>
-      <c r="H35" s="38">
+      <c r="H35" s="40">
         <v>43231.24336197917</v>
       </c>
       <c r="I35" t="s">
@@ -4902,7 +4913,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -4924,7 +4935,7 @@
       <c r="G36" t="s">
         <v>80</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="40">
         <v>43231.245057939814</v>
       </c>
       <c r="I36" t="s">
@@ -4985,7 +4996,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -5007,8 +5018,8 @@
       <c r="G37" t="s">
         <v>119</v>
       </c>
-      <c r="H37" s="38">
-        <v>43231.249065127311</v>
+      <c r="H37" s="40">
+        <v>43231.24906512731</v>
       </c>
       <c r="I37" t="s">
         <v>93</v>
@@ -5068,7 +5079,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -5090,8 +5101,8 @@
       <c r="G38" t="s">
         <v>121</v>
       </c>
-      <c r="H38" s="38">
-        <v>43231.256770069449</v>
+      <c r="H38" s="40">
+        <v>43231.25677006945</v>
       </c>
       <c r="I38" t="s">
         <v>81</v>
@@ -5151,7 +5162,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -5173,7 +5184,7 @@
       <c r="G39" t="s">
         <v>119</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="40">
         <v>43231.258041099536</v>
       </c>
       <c r="I39" t="s">
@@ -5234,7 +5245,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -5256,8 +5267,8 @@
       <c r="G40" t="s">
         <v>119</v>
       </c>
-      <c r="H40" s="38">
-        <v>43231.260167129629</v>
+      <c r="H40" s="40">
+        <v>43231.26016712963</v>
       </c>
       <c r="I40" t="s">
         <v>81</v>
@@ -5317,7 +5328,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -5339,8 +5350,8 @@
       <c r="G41" t="s">
         <v>119</v>
       </c>
-      <c r="H41" s="38">
-        <v>43231.262908738427</v>
+      <c r="H41" s="40">
+        <v>43231.26290873843</v>
       </c>
       <c r="I41" t="s">
         <v>81</v>
@@ -5400,7 +5411,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:27">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -5422,7 +5433,7 @@
       <c r="G42" t="s">
         <v>121</v>
       </c>
-      <c r="H42" s="38">
+      <c r="H42" s="40">
         <v>43231.263154722226</v>
       </c>
       <c r="I42" t="s">
@@ -5483,7 +5494,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -5505,8 +5516,8 @@
       <c r="G43" t="s">
         <v>119</v>
       </c>
-      <c r="H43" s="38">
-        <v>43231.263997858798</v>
+      <c r="H43" s="40">
+        <v>43231.2639978588</v>
       </c>
       <c r="I43" t="s">
         <v>81</v>
@@ -5566,7 +5577,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -5588,8 +5599,8 @@
       <c r="G44" t="s">
         <v>119</v>
       </c>
-      <c r="H44" s="38">
-        <v>43231.266265532409</v>
+      <c r="H44" s="40">
+        <v>43231.26626553241</v>
       </c>
       <c r="I44" t="s">
         <v>93</v>
@@ -5649,7 +5660,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -5671,8 +5682,8 @@
       <c r="G45" t="s">
         <v>119</v>
       </c>
-      <c r="H45" s="38">
-        <v>43231.267808182871</v>
+      <c r="H45" s="40">
+        <v>43231.26780818287</v>
       </c>
       <c r="I45" t="s">
         <v>136</v>
@@ -5732,7 +5743,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -5754,7 +5765,7 @@
       <c r="G46" t="s">
         <v>119</v>
       </c>
-      <c r="H46" s="38">
+      <c r="H46" s="40">
         <v>43231.268242210645</v>
       </c>
       <c r="I46" t="s">
@@ -5815,7 +5826,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>64</v>
       </c>
@@ -5837,8 +5848,8 @@
       <c r="G47" t="s">
         <v>119</v>
       </c>
-      <c r="H47" s="38">
-        <v>43231.268848749998</v>
+      <c r="H47" s="40">
+        <v>43231.26884875</v>
       </c>
       <c r="I47" t="s">
         <v>95</v>
@@ -5898,7 +5909,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -5920,8 +5931,8 @@
       <c r="G48" t="s">
         <v>119</v>
       </c>
-      <c r="H48" s="38">
-        <v>43231.269386574073</v>
+      <c r="H48" s="40">
+        <v>43231.26938657407</v>
       </c>
       <c r="I48" t="s">
         <v>136</v>
@@ -5978,6 +5989,172 @@
         <v>76</v>
       </c>
       <c r="AA48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" t="s">
+        <v>143</v>
+      </c>
+      <c r="G49" t="s">
+        <v>119</v>
+      </c>
+      <c r="H49" s="40">
+        <v>43231.275544212964</v>
+      </c>
+      <c r="I49" t="s">
+        <v>95</v>
+      </c>
+      <c r="J49" t="s">
+        <v>76</v>
+      </c>
+      <c r="K49" t="s">
+        <v>144</v>
+      </c>
+      <c r="L49" t="s">
+        <v>76</v>
+      </c>
+      <c r="M49" t="s">
+        <v>76</v>
+      </c>
+      <c r="N49" t="s">
+        <v>76</v>
+      </c>
+      <c r="O49" t="s">
+        <v>76</v>
+      </c>
+      <c r="P49" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>76</v>
+      </c>
+      <c r="R49" t="s">
+        <v>76</v>
+      </c>
+      <c r="S49" t="s">
+        <v>76</v>
+      </c>
+      <c r="T49" t="s">
+        <v>76</v>
+      </c>
+      <c r="U49" t="s">
+        <v>76</v>
+      </c>
+      <c r="V49" t="s">
+        <v>76</v>
+      </c>
+      <c r="W49" t="s">
+        <v>76</v>
+      </c>
+      <c r="X49" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" t="s">
+        <v>145</v>
+      </c>
+      <c r="G50" t="s">
+        <v>119</v>
+      </c>
+      <c r="H50" s="40">
+        <v>43231.29015115741</v>
+      </c>
+      <c r="I50" t="s">
+        <v>81</v>
+      </c>
+      <c r="J50" t="s">
+        <v>76</v>
+      </c>
+      <c r="K50" t="s">
+        <v>146</v>
+      </c>
+      <c r="L50" t="s">
+        <v>76</v>
+      </c>
+      <c r="M50" t="s">
+        <v>76</v>
+      </c>
+      <c r="N50" t="s">
+        <v>76</v>
+      </c>
+      <c r="O50" t="s">
+        <v>76</v>
+      </c>
+      <c r="P50" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>76</v>
+      </c>
+      <c r="R50" t="s">
+        <v>76</v>
+      </c>
+      <c r="S50" t="s">
+        <v>76</v>
+      </c>
+      <c r="T50" t="s">
+        <v>76</v>
+      </c>
+      <c r="U50" t="s">
+        <v>76</v>
+      </c>
+      <c r="V50" t="s">
+        <v>76</v>
+      </c>
+      <c r="W50" t="s">
+        <v>76</v>
+      </c>
+      <c r="X50" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA50" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>